<commit_message>
revision of objective and proposal
</commit_message>
<xml_diff>
--- a/AMBAGAN.xlsx
+++ b/AMBAGAN.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2B7BAB-B834-400B-89B4-229F325275D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1419DAF-AB0C-4FA7-B577-D1431AA8B9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F381F51-3A00-4C97-8965-4FFDADBDCF80}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Expenses" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,74 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">
-1. Research sa theory how magnet fields work + ung trial ng mga iba na tinatry maachieve ung "free energy" 
-2. itest ung theory on small scale (ung fidget spinner + arbitrarily positioned magnets) 
-3.)  if oke ang test, magdesign na ng actual design natin
-3.1) IF HINDI okay ang test, edi balik sa 1.
-3.2) pag hindi talaga kaya, proceed tayo sa plan C (servo motor)
-4.) proceed sa paggawa ng the rest (with documentation)</t>
-  </si>
-  <si>
-    <t>For number 2 (testing stage):</t>
-  </si>
-  <si>
-    <t>example scenario: ung candidate number 1 magnet</t>
-  </si>
-  <si>
-    <t>if ung binili ko (given that it has a variation sa quantity (eg. Ung candidate number 1 ng magnets))</t>
-  </si>
-  <si>
-    <t>wasn't used for testing and/or the final output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">then I wont charge </t>
-  </si>
-  <si>
-    <t>was used partially (eg. 1 to 10 pieces for testing and/or final output)</t>
-  </si>
-  <si>
-    <t>I will charge the "10 variation" for the product</t>
-  </si>
-  <si>
-    <t>was used partially (eg. 11 to 20 pieces for testing and/or final output)</t>
-  </si>
-  <si>
-    <t>I will charge the "20 variation" for the product</t>
-  </si>
-  <si>
-    <t>was used partially (eg. 21 to 50 pieces for testing and/or final output)</t>
-  </si>
-  <si>
-    <t>I will charge the "50 variation" for the product</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>candidate 1 magnet</t>
+  </si>
+  <si>
+    <t>no.</t>
+  </si>
+  <si>
+    <t>item name</t>
+  </si>
+  <si>
+    <t>candidate 2 magnet</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price </t>
+  </si>
+  <si>
+    <t>total with shipping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,17 +77,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,103 +412,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F572D62-4C01-4AE7-8A1A-8AFAE522E495}">
-  <dimension ref="B3:K26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3A88E5-1C2E-4E37-BE69-6396071FF29A}">
+  <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="6" spans="2:11" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B6" s="2" t="s">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B7" s="3" t="s">
+      <c r="D3" s="1">
+        <v>239</v>
+      </c>
+      <c r="E3" s="1">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="D4" s="1">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:K3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>